<commit_message>
Added functional test for simulator
</commit_message>
<xml_diff>
--- a/templates/dev_templates.xlsx
+++ b/templates/dev_templates.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\dev\iap\dev_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\dev\iap\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2420,8 +2420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N629"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A340" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I347" sqref="I347"/>
+    <sheetView tabSelected="1" topLeftCell="A341" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G349" sqref="G349"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11088,7 +11088,7 @@
       </c>
       <c r="F349" s="8"/>
       <c r="G349" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H349" s="8"/>
       <c r="I349" s="8"/>

</xml_diff>